<commit_message>
Sensor data sheets and application notes
Uploaded data sheets for IR LED and photo transistor along with
application notes from Fairchild Semiconductor on designing a photo
interrupt amplifier circuit
</commit_message>
<xml_diff>
--- a/BOM/MasterBOM.xlsx
+++ b/BOM/MasterBOM.xlsx
@@ -218,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -227,6 +227,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -529,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,7 +712,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -732,8 +734,38 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="5">
         <f>SUM(D3,D5,D6,D7,D8)</f>
         <v>49.55</v>
       </c>

</xml_diff>